<commit_message>
Changed network_b worksheet to threshold_b
</commit_message>
<xml_diff>
--- a/test_files/forward_tests/4-genes_6-edges_artificial-data_Sigmoid_forward.xlsx
+++ b/test_files/forward_tests/4-genes_6-edges_artificial-data_Sigmoid_forward.xlsx
@@ -14,7 +14,7 @@
     <sheet name="network" sheetId="5" r:id="rId5"/>
     <sheet name="network_weights" sheetId="11" r:id="rId6"/>
     <sheet name="optimization_parameters" sheetId="6" r:id="rId7"/>
-    <sheet name="network_b" sheetId="16" r:id="rId8"/>
+    <sheet name="threshold_b" sheetId="16" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">network!$A$1:$V$22</definedName>
@@ -2055,7 +2055,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated names of worksheets to reflect issue#88
</commit_message>
<xml_diff>
--- a/test_files/forward_tests/4-genes_6-edges_artificial-data_Sigmoid_forward.xlsx
+++ b/test_files/forward_tests/4-genes_6-edges_artificial-data_Sigmoid_forward.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="25605" windowHeight="16005" tabRatio="644" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="510" yWindow="-30" windowWidth="20220" windowHeight="10920" tabRatio="644" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
     <sheet name="degradation_rates" sheetId="1" r:id="rId2"/>
-    <sheet name="wt" sheetId="17" r:id="rId3"/>
-    <sheet name="dcin5" sheetId="18" r:id="rId4"/>
+    <sheet name="wt_log2_expression" sheetId="17" r:id="rId3"/>
+    <sheet name="dcin5_log2_expression" sheetId="18" r:id="rId4"/>
     <sheet name="network" sheetId="5" r:id="rId5"/>
     <sheet name="network_weights" sheetId="11" r:id="rId6"/>
     <sheet name="optimization_parameters" sheetId="6" r:id="rId7"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">network!$A$1:$V$22</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>

</xml_diff>